<commit_message>
NICK MF Reporting: - new Sing GL excel form - new NOAL form - some code refactoring and bug fixing
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_7.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_7.xlsx
@@ -15,9 +15,9 @@
     <sheet name="РФИ_7" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="GR_CODE_ROW">4583</definedName>
     <definedName name="GR_CODE_SHEET">4</definedName>
-    <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">РФИ_7!$A$1:$AN$40</definedName>
   </definedNames>
   <calcPr calcId="152511" iterate="1"/>
@@ -121,36 +121,6 @@
   </si>
   <si>
     <t>Резервы на покрытие убытков</t>
-  </si>
-  <si>
-    <t>Итого балансовая стоимость (гр. 11+гр.12+гр.13+гр.14+гр.15+гр.16+гр.17)</t>
-  </si>
-  <si>
-    <t>Количество (гр.10+гр.19)</t>
-  </si>
-  <si>
-    <t>Сумма основного долга/номинальная стоимость (гр.11+гр.20)</t>
-  </si>
-  <si>
-    <t>Дисконт (гр.12+гр.21)</t>
-  </si>
-  <si>
-    <t>Премия (гр.13+гр.22)</t>
-  </si>
-  <si>
-    <t>Вознаграждение (гр.14+гр.23)</t>
-  </si>
-  <si>
-    <t>Вознаграждение предыдущего держателя (гр.15+гр.24)</t>
-  </si>
-  <si>
-    <t>Корректировка справедливой стоимости (гр.16+гр.25+гр.26)</t>
-  </si>
-  <si>
-    <t>Резервы на покрытие убытков (гр.17+гр.27)</t>
-  </si>
-  <si>
-    <t>Итого балансовая стоимость (гр.29+гр.30+гр.31+гр.32+гр.33+гр.34+гр.35)</t>
   </si>
   <si>
     <t>положительная</t>
@@ -330,11 +300,41 @@
   <si>
     <t>Валюта</t>
   </si>
+  <si>
+    <t>Итого балансовая стоимость (гр.12+гр.13+гр.14+гр.15+гр.16+гр.17+гр.18)</t>
+  </si>
+  <si>
+    <t>Количество (гр.11+гр.20)</t>
+  </si>
+  <si>
+    <t>Сумма основного долга/номинальная стоимость (гр.12+гр.21)</t>
+  </si>
+  <si>
+    <t>Дисконт (гр.13+гр.22)</t>
+  </si>
+  <si>
+    <t>Премия (гр.14+гр.23)</t>
+  </si>
+  <si>
+    <t>Вознаграждение (гр.15+гр.24)</t>
+  </si>
+  <si>
+    <t>Вознаграждение предыдущего держателя (гр.16+гр.25)</t>
+  </si>
+  <si>
+    <t>Корректировка справедливой стоимости (гр.17+гр.26+гр.27)</t>
+  </si>
+  <si>
+    <t>Резервы на покрытие убытков (гр.18+гр.28)</t>
+  </si>
+  <si>
+    <t>Итого балансовая стоимость (гр.30+гр.31+гр.32+гр.33+гр.34+гр.35+гр.36)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000000"/>
@@ -689,80 +689,80 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 7" xfId="2"/>
     <cellStyle name="Обычный_ФормОтчет" xfId="3"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1079,10 +1079,10 @@
   </sheetPr>
   <dimension ref="A1:AS83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="AE1" activePane="topRight" state="frozen"/>
       <selection activeCell="H83" sqref="H83"/>
-      <selection pane="topRight" activeCell="AK17" sqref="AK17"/>
+      <selection pane="topRight" activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="50" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3494,92 +3494,92 @@
       <c r="AN8" s="1"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
-      <c r="U9" s="73"/>
-      <c r="V9" s="73"/>
-      <c r="W9" s="73"/>
-      <c r="X9" s="73"/>
-      <c r="Y9" s="73"/>
-      <c r="Z9" s="73"/>
-      <c r="AA9" s="73"/>
-      <c r="AB9" s="73"/>
-      <c r="AC9" s="73"/>
-      <c r="AD9" s="73"/>
-      <c r="AE9" s="73"/>
-      <c r="AF9" s="73"/>
-      <c r="AG9" s="73"/>
-      <c r="AH9" s="73"/>
-      <c r="AI9" s="73"/>
-      <c r="AJ9" s="73"/>
-      <c r="AK9" s="73"/>
-      <c r="AL9" s="73"/>
-      <c r="AM9" s="73"/>
-      <c r="AN9" s="73"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
+      <c r="V9" s="56"/>
+      <c r="W9" s="56"/>
+      <c r="X9" s="56"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="56"/>
+      <c r="AB9" s="56"/>
+      <c r="AC9" s="56"/>
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56"/>
+      <c r="AF9" s="56"/>
+      <c r="AG9" s="56"/>
+      <c r="AH9" s="56"/>
+      <c r="AI9" s="56"/>
+      <c r="AJ9" s="56"/>
+      <c r="AK9" s="56"/>
+      <c r="AL9" s="56"/>
+      <c r="AM9" s="56"/>
+      <c r="AN9" s="56"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73"/>
-      <c r="T10" s="73"/>
-      <c r="U10" s="73"/>
-      <c r="V10" s="73"/>
-      <c r="W10" s="73"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-      <c r="Z10" s="73"/>
-      <c r="AA10" s="73"/>
-      <c r="AB10" s="73"/>
-      <c r="AC10" s="73"/>
-      <c r="AD10" s="73"/>
-      <c r="AE10" s="73"/>
-      <c r="AF10" s="73"/>
-      <c r="AG10" s="73"/>
-      <c r="AH10" s="73"/>
-      <c r="AI10" s="73"/>
-      <c r="AJ10" s="73"/>
-      <c r="AK10" s="73"/>
-      <c r="AL10" s="73"/>
-      <c r="AM10" s="73"/>
-      <c r="AN10" s="73"/>
+      <c r="A10" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="56"/>
+      <c r="V10" s="56"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="56"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="56"/>
+      <c r="AB10" s="56"/>
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56"/>
+      <c r="AF10" s="56"/>
+      <c r="AG10" s="56"/>
+      <c r="AH10" s="56"/>
+      <c r="AI10" s="56"/>
+      <c r="AJ10" s="56"/>
+      <c r="AK10" s="56"/>
+      <c r="AL10" s="56"/>
+      <c r="AM10" s="56"/>
+      <c r="AN10" s="56"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -3666,209 +3666,209 @@
       <c r="AN12" s="1"/>
     </row>
     <row r="13" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="64" t="s">
+      <c r="E13" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="64" t="s">
+      <c r="F13" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="64" t="s">
+      <c r="G13" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="64" t="s">
+      <c r="H13" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="64" t="s">
+      <c r="I13" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13" s="67" t="s">
+      <c r="J13" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="68"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="70" t="s">
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="72"/>
+      <c r="Q13" s="72"/>
+      <c r="R13" s="72"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="U13" s="71"/>
-      <c r="V13" s="71"/>
-      <c r="W13" s="71"/>
-      <c r="X13" s="71"/>
-      <c r="Y13" s="71"/>
-      <c r="Z13" s="71"/>
-      <c r="AA13" s="71"/>
-      <c r="AB13" s="72"/>
-      <c r="AC13" s="67" t="s">
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="74"/>
+      <c r="X13" s="74"/>
+      <c r="Y13" s="74"/>
+      <c r="Z13" s="74"/>
+      <c r="AA13" s="74"/>
+      <c r="AB13" s="75"/>
+      <c r="AC13" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AD13" s="68"/>
-      <c r="AE13" s="68"/>
-      <c r="AF13" s="68"/>
-      <c r="AG13" s="68"/>
-      <c r="AH13" s="68"/>
-      <c r="AI13" s="68"/>
-      <c r="AJ13" s="68"/>
-      <c r="AK13" s="69"/>
+      <c r="AD13" s="72"/>
+      <c r="AE13" s="72"/>
+      <c r="AF13" s="72"/>
+      <c r="AG13" s="72"/>
+      <c r="AH13" s="72"/>
+      <c r="AI13" s="72"/>
+      <c r="AJ13" s="72"/>
+      <c r="AK13" s="66"/>
       <c r="AL13" s="7"/>
       <c r="AM13" s="8"/>
       <c r="AN13" s="8"/>
     </row>
     <row r="14" spans="1:40" s="9" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="64" t="s">
+      <c r="A14" s="58"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="64" t="s">
+      <c r="L14" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="64" t="s">
+      <c r="M14" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="64" t="s">
+      <c r="N14" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="64" t="s">
+      <c r="O14" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="64" t="s">
+      <c r="P14" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="Q14" s="64" t="s">
+      <c r="Q14" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="R14" s="64" t="s">
+      <c r="R14" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="S14" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="T14" s="64" t="s">
+      <c r="S14" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="T14" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="U14" s="64" t="s">
+      <c r="U14" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="V14" s="64" t="s">
+      <c r="V14" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="W14" s="64" t="s">
+      <c r="W14" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="X14" s="64" t="s">
+      <c r="X14" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="Y14" s="64" t="s">
+      <c r="Y14" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="Z14" s="67" t="s">
+      <c r="Z14" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="64" t="s">
+      <c r="AA14" s="66"/>
+      <c r="AB14" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="AC14" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD14" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE14" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF14" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG14" s="64" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH14" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI14" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ14" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK14" s="64" t="s">
-        <v>39</v>
+      <c r="AC14" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD14" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE14" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF14" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG14" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH14" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI14" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ14" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK14" s="60" t="s">
+        <v>63</v>
       </c>
       <c r="AL14" s="7"/>
       <c r="AM14" s="10"/>
       <c r="AN14" s="10"/>
     </row>
     <row r="15" spans="1:40" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="65"/>
-      <c r="S15" s="65"/>
-      <c r="T15" s="65"/>
-      <c r="U15" s="65"/>
-      <c r="V15" s="65"/>
-      <c r="W15" s="65"/>
-      <c r="X15" s="65"/>
-      <c r="Y15" s="65"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="62"/>
+      <c r="W15" s="62"/>
+      <c r="X15" s="62"/>
+      <c r="Y15" s="62"/>
       <c r="Z15" s="11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AA15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB15" s="65"/>
-      <c r="AC15" s="65"/>
-      <c r="AD15" s="65"/>
-      <c r="AE15" s="65"/>
-      <c r="AF15" s="65"/>
-      <c r="AG15" s="65"/>
-      <c r="AH15" s="65"/>
-      <c r="AI15" s="65"/>
-      <c r="AJ15" s="65"/>
-      <c r="AK15" s="65"/>
+        <v>31</v>
+      </c>
+      <c r="AB15" s="62"/>
+      <c r="AC15" s="62"/>
+      <c r="AD15" s="62"/>
+      <c r="AE15" s="62"/>
+      <c r="AF15" s="62"/>
+      <c r="AG15" s="62"/>
+      <c r="AH15" s="62"/>
+      <c r="AI15" s="62"/>
+      <c r="AJ15" s="62"/>
+      <c r="AK15" s="62"/>
       <c r="AL15" s="7"/>
       <c r="AM15" s="10"/>
       <c r="AN15" s="10"/>
@@ -3991,8 +3991,8 @@
     </row>
     <row r="17" spans="1:45" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="77" t="s">
-        <v>57</v>
+      <c r="B17" s="55" t="s">
+        <v>47</v>
       </c>
       <c r="C17" s="15">
         <v>1</v>
@@ -4038,7 +4038,7 @@
     <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C18" s="15">
         <v>2</v>
@@ -4084,7 +4084,7 @@
     <row r="19" spans="1:45" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C19" s="15">
         <v>3</v>
@@ -4130,7 +4130,7 @@
     <row r="20" spans="1:45" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C20" s="15">
         <v>4</v>
@@ -4176,7 +4176,7 @@
     <row r="21" spans="1:45" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C21" s="15">
         <v>5</v>
@@ -4222,7 +4222,7 @@
     <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C22" s="15">
         <v>6</v>
@@ -4268,7 +4268,7 @@
     <row r="23" spans="1:45" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C23" s="15">
         <v>7</v>
@@ -4312,7 +4312,7 @@
     <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C24" s="15">
         <v>8</v>
@@ -4358,7 +4358,7 @@
     <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C25" s="15">
         <v>9</v>
@@ -4404,7 +4404,7 @@
     <row r="26" spans="1:45" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C26" s="15">
         <v>10</v>
@@ -4453,7 +4453,7 @@
     <row r="27" spans="1:45" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
       <c r="B27" s="14" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C27" s="34">
         <v>11</v>
@@ -4503,7 +4503,7 @@
     <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="14" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C28" s="34">
         <v>12</v>
@@ -4553,7 +4553,7 @@
     <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
       <c r="B29" s="14" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C29" s="34">
         <v>13</v>
@@ -4597,10 +4597,10 @@
       <c r="AN29" s="25"/>
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A30" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="62"/>
+      <c r="A30" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="68"/>
       <c r="C30" s="15">
         <v>14</v>
       </c>
@@ -4686,18 +4686,18 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
+      <c r="B32" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -4730,18 +4730,18 @@
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
+      <c r="B33" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -4774,18 +4774,18 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
+      <c r="B34" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -4818,18 +4818,18 @@
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
+      <c r="B35" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -4862,18 +4862,18 @@
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
+      <c r="B36" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -4907,7 +4907,7 @@
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="40" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C37" s="41"/>
       <c r="D37" s="41"/>
@@ -4950,18 +4950,18 @@
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="58"/>
+      <c r="B38" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -4994,18 +4994,18 @@
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="60"/>
+      <c r="B39" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
+      <c r="K39" s="77"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -5038,18 +5038,18 @@
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="60"/>
-      <c r="J40" s="60"/>
-      <c r="K40" s="60"/>
+      <c r="B40" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="77"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="77"/>
+      <c r="J40" s="77"/>
+      <c r="K40" s="77"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -5104,100 +5104,100 @@
       <c r="AJ42" s="27"/>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="76"/>
       <c r="Q43" s="27"/>
       <c r="AJ43" s="27"/>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="76"/>
       <c r="Q44" s="27"/>
       <c r="AJ44" s="27"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
       <c r="Q45" s="27"/>
       <c r="AJ45" s="27"/>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="76"/>
+      <c r="I46" s="76"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="76"/>
       <c r="Q46" s="27"/>
       <c r="AJ46" s="27"/>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
       <c r="Q47" s="27"/>
       <c r="AJ47" s="27"/>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
-      <c r="J48" s="56"/>
-      <c r="K48" s="56"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="63"/>
       <c r="Q48" s="27"/>
       <c r="AJ48" s="27"/>
     </row>
     <row r="49" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="55"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="76"/>
       <c r="Q49" s="27"/>
       <c r="AJ49" s="27"/>
     </row>
@@ -5320,19 +5320,34 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="A9:AN9"/>
-    <mergeCell ref="A10:AN10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="AJ14:AJ15"/>
-    <mergeCell ref="AK14:AK15"/>
-    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="B49:K49"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B36:K36"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="B48:K48"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="AH14:AH15"/>
+    <mergeCell ref="AI14:AI15"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="K13:S13"/>
+    <mergeCell ref="T13:AB13"/>
+    <mergeCell ref="AC13:AK13"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
     <mergeCell ref="B34:K34"/>
     <mergeCell ref="AD14:AD15"/>
     <mergeCell ref="AE14:AE15"/>
@@ -5349,34 +5364,19 @@
     <mergeCell ref="S14:S15"/>
     <mergeCell ref="T14:T15"/>
     <mergeCell ref="U14:U15"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="AH14:AH15"/>
-    <mergeCell ref="AI14:AI15"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="K13:S13"/>
-    <mergeCell ref="T13:AB13"/>
-    <mergeCell ref="AC13:AK13"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="B49:K49"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:K36"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="B48:K48"/>
+    <mergeCell ref="A9:AN9"/>
+    <mergeCell ref="A10:AN10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="AJ14:AJ15"/>
+    <mergeCell ref="AK14:AK15"/>
+    <mergeCell ref="J13:J15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="55" orientation="landscape" r:id="rId1"/>

</xml_diff>